<commit_message>
Finalizado os cards do frontend
</commit_message>
<xml_diff>
--- a/Códigos - Popular base/Flávia/matchIds.xlsx
+++ b/Códigos - Popular base/Flávia/matchIds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flavia.de.oliveira\Documents\TCC\Códigos - Popular base\Flávia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D53FF1-BF5A-4837-8770-F9329DB5DF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAAE816-F3AD-4B4C-8EA5-344094C4386F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9496,7 +9496,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9506,6 +9506,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9537,34 +9543,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEBF1DE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDAEEF3"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -9864,7 +9854,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A3151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -9877,12 +9869,12 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>